<commit_message>
Only use today's files and add platform name as a variable.
</commit_message>
<xml_diff>
--- a/src/krbiz/_resources/_order_delivery_config_template.xlsx
+++ b/src/krbiz/_resources/_order_delivery_config_template.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10917"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunyoungyoo/Desktop/krbiz/src/krbiz/_resources/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334A5049-3B89-6A4A-B7FF-2E845AE929C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="20760" yWindow="11720" windowWidth="28260" windowHeight="9180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="variable_mapping"/>
-    <sheet r:id="rId2" sheetId="2" name="CJ"/>
+    <sheet name="variable_mapping" sheetId="1" r:id="rId1"/>
+    <sheet name="LOTTE" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
   <si>
     <t>받는분성명</t>
   </si>
@@ -47,9 +53,7 @@
     <t>{receipients_phone_number}</t>
   </si>
   <si>
-    <t>{long_address},
-{short_address}
-{additional_address}</t>
+    <t>{long_address}</t>
   </si>
   <si>
     <t>{product_name}</t>
@@ -61,10 +65,13 @@
     <t>{message}</t>
   </si>
   <si>
+    <t>{PlatformName}</t>
+  </si>
+  <si>
     <t>{order_id}</t>
   </si>
   <si>
-    <t>Name</t>
+    <t>Platform Name</t>
   </si>
   <si>
     <t>Header Row</t>
@@ -181,21 +188,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -213,7 +213,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFdddddd"/>
+        <fgColor rgb="FFDDDDDD"/>
       </patternFill>
     </fill>
   </fills>
@@ -245,7 +245,7 @@
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color rgb="FFc6c6c6"/>
+        <color rgb="FFC6C6C6"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
@@ -266,50 +266,47 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+  <cellXfs count="10">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -320,10 +317,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -361,71 +358,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -453,7 +450,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -476,11 +473,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -489,13 +486,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -505,7 +502,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -514,7 +511,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -523,7 +520,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -531,10 +528,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -599,168 +596,168 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="9" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="16.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="7" width="16.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="7" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="7" width="20.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="7" width="20.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="7" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="7" width="25.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="7" width="16.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="7" width="18.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="7" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.33203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.5" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" s="10" t="s">
+    <row r="1" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>16</v>
       </c>
+      <c r="B1" s="8" t="s">
+        <v>17</v>
+      </c>
       <c r="C1" s="4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O1" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
-      <c r="A2" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="B2" s="10">
+    <row r="2" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="8">
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
       <c r="L2" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
-      <c r="A3" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B3" s="10">
+    <row r="3" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="8">
         <v>2</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="O3" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -769,27 +766,29 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" style="7" width="19.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="28.005" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="27.14785714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="18.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="13.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="9" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="9" width="44.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="19.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="44.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row r="1" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -815,7 +814,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
+    <row r="2" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -825,18 +824,20 @@
       <c r="C2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6" t="s">
+      <c r="G2" t="s">
         <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add more platforms as default.
</commit_message>
<xml_diff>
--- a/src/krbiz/_resources/_order_delivery_config_template.xlsx
+++ b/src/krbiz/_resources/_order_delivery_config_template.xlsx
@@ -1,27 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10917"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sunyoungyoo/Desktop/krbiz/src/krbiz/_resources/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{334A5049-3B89-6A4A-B7FF-2E845AE929C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20760" yWindow="11720" windowWidth="28260" windowHeight="9180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="variable_mapping" sheetId="1" r:id="rId1"/>
-    <sheet name="LOTTE" sheetId="2" r:id="rId2"/>
+    <sheet r:id="rId1" sheetId="1" name="variable_mapping"/>
+    <sheet r:id="rId2" sheetId="2" name="LOTTE"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="71">
   <si>
     <t>받는분성명</t>
   </si>
@@ -116,7 +110,7 @@
     <t>product_id</t>
   </si>
   <si>
-    <t>Coupang</t>
+    <t>Gmarket</t>
   </si>
   <si>
     <t>주문번호</t>
@@ -150,6 +144,57 @@
   </si>
   <si>
     <t>상품번호</t>
+  </si>
+  <si>
+    <t>Wadiz</t>
+  </si>
+  <si>
+    <t>주문 번호</t>
+  </si>
+  <si>
+    <t>주문 상품</t>
+  </si>
+  <si>
+    <t>주문 옵션</t>
+  </si>
+  <si>
+    <t>주문 수량</t>
+  </si>
+  <si>
+    <t>받는 분</t>
+  </si>
+  <si>
+    <t>배송지 우편번호</t>
+  </si>
+  <si>
+    <t>배송지 주소</t>
+  </si>
+  <si>
+    <t>받는 분 연락처</t>
+  </si>
+  <si>
+    <t>서포터 연락처</t>
+  </si>
+  <si>
+    <t>배송 요청 사항</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>11TH</t>
+  </si>
+  <si>
+    <t>옵션</t>
+  </si>
+  <si>
+    <t>수취인</t>
+  </si>
+  <si>
+    <t>휴대폰번호</t>
+  </si>
+  <si>
+    <t>배송메시지</t>
   </si>
   <si>
     <t>Naver</t>
@@ -188,7 +233,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -213,7 +259,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFDDDDDD"/>
+        <fgColor rgb="FFdddddd"/>
       </patternFill>
     </fill>
   </fills>
@@ -245,7 +291,7 @@
         <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color rgb="FFC6C6C6"/>
+        <color rgb="FFc6c6c6"/>
       </right>
       <top style="thin">
         <color rgb="FF000000"/>
@@ -266,47 +312,59 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="15">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -317,10 +375,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -358,71 +416,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -450,7 +508,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -473,11 +531,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -486,13 +544,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -502,7 +560,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -511,7 +569,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -520,7 +578,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -528,10 +586,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -596,38 +654,38 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:O5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.1640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.83203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.33203125" style="6" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="9" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="14" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="17.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="7" width="23.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="7" width="16.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="7" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="7" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="7" width="20.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="7" width="20.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="7" width="12.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="12" max="12" style="7" width="25.862142857142857" customWidth="1" bestFit="1"/>
+    <col min="13" max="13" style="7" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" style="7" width="18.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="15" max="15" style="7" width="12.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+      <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>17</v>
       </c>
       <c r="C1" s="4" t="s">
@@ -670,11 +728,11 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
+      <c r="A2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="8">
+      <c r="B2" s="10">
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
@@ -713,51 +771,139 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="17.25">
+      <c r="A3" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="11">
+        <v>1</v>
+      </c>
+      <c r="C3" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="O3" s="13" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="17.25">
+      <c r="A4" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="11">
         <v>2</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="4" t="s">
+      <c r="C4" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="E4" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="H3" s="4" t="s">
+      <c r="G4" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="H4" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="K3" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="N3" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>53</v>
+      <c r="I4" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="N4" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="O4" s="12" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
+      <c r="A5" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5" s="10">
+        <v>2</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="K5" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="L5" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="M5" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="N5" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -766,29 +912,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5" style="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="44.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="7" width="19.719285714285714" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="7" width="28.005" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="8" width="24.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="7" width="18.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="9" width="13.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="9" width="22.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="9" width="44.57642857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="20.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -814,7 +958,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
@@ -824,19 +968,19 @@
       <c r="C2" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="6" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="6" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add coupang as a supported platform.
</commit_message>
<xml_diff>
--- a/src/krbiz/_resources/_order_delivery_config_template.xlsx
+++ b/src/krbiz/_resources/_order_delivery_config_template.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="80">
   <si>
     <t>받는분성명</t>
   </si>
@@ -197,6 +197,36 @@
     <t>배송메시지</t>
   </si>
   <si>
+    <t>Coupang</t>
+  </si>
+  <si>
+    <t>등록상품명</t>
+  </si>
+  <si>
+    <t>등록옵션명</t>
+  </si>
+  <si>
+    <t>구매수(수량)</t>
+  </si>
+  <si>
+    <t>수취인이름</t>
+  </si>
+  <si>
+    <t>수취인 주소</t>
+  </si>
+  <si>
+    <t>수취인전화번호</t>
+  </si>
+  <si>
+    <t>구매자전화번호</t>
+  </si>
+  <si>
+    <t>배송메세지</t>
+  </si>
+  <si>
+    <t>노출상품ID</t>
+  </si>
+  <si>
     <t>Naver</t>
   </si>
   <si>
@@ -222,9 +252,6 @@
   </si>
   <si>
     <t>수취인연락처2</t>
-  </si>
-  <si>
-    <t>배송메세지</t>
   </si>
   <si>
     <t>옵션관리코드</t>
@@ -658,7 +685,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -859,51 +886,94 @@
         <v>42</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="17.25">
       <c r="A5" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="B5" s="10">
+      <c r="B5" s="11">
+        <v>1</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="H5" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="M5" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="N5" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="O5" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
+      <c r="A6" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B6" s="10">
         <v>2</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="C6" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F5" s="4" t="s">
+      <c r="E6" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="H5" s="4" t="s">
+      <c r="G6" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="I5" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="K5" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="L5" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="M5" s="4" t="s">
+      <c r="I6" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="M6" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="N6" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="N5" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>70</v>
+      <c r="O6" s="4" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>